<commit_message>
Ateco 2007- aggiornamento 2022 (#49)
* ateco2007-2022

modifica prefLabel nel file ttl

* ateco2007-2022

modifiche prefLabel e modified nel file ttl

* aggiornamento ateco

modifica metadati ateco2007-2022 ed eliminazione di ateco2025

* ateco2007-2022

eliminazione :B dal file ttl

* ateco2007-2022

Rimozione cronologia ateco file ttl

* Ateco2007-2022

Caricamento files per Ateco 2007- aggiornamento 2022
</commit_message>
<xml_diff>
--- a/assets/controlled-vocabularies/classifications-for-organizations/ateco-2007-2022/ateco-2007-2022.xlsx
+++ b/assets/controlled-vocabularies/classifications-for-organizations/ateco-2007-2022/ateco-2007-2022.xlsx
@@ -41234,8 +41234,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010072D98D2D97F681408BF953384BD5A9A3" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="12dd57c485e34d55deca9cda06702448">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="90fcb089-f94f-4bc2-91e5-43965b06e971" xmlns:ns3="c85358b1-421f-4fd0-879b-9050862305dc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0ce440a7e8cd611422ddaf574cf90f1d" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010072D98D2D97F681408BF953384BD5A9A3" ma:contentTypeVersion="12" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="eb49e0e161572593fea98bb69e68ac17">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="90fcb089-f94f-4bc2-91e5-43965b06e971" xmlns:ns3="c85358b1-421f-4fd0-879b-9050862305dc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9ca9ed287faa8d1eb8a7c0115ec2669a" ns2:_="" ns3:_="">
     <xsd:import namespace="90fcb089-f94f-4bc2-91e5-43965b06e971"/>
     <xsd:import namespace="c85358b1-421f-4fd0-879b-9050862305dc"/>
     <xsd:element name="properties">
@@ -41305,7 +41305,7 @@
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="17" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="2187dd90-94de-4f52-8f02-9967864c5993" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="17" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Tag immagine" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="2187dd90-94de-4f52-8f02-9967864c5993" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -41344,8 +41344,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo di contenuto"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titolo"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -41463,7 +41463,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E90B1926-69AD-441B-B84A-B8BBC9C0D429}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3FC7B5D1-282A-4EA2-B61F-6AC6C82B8A07}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>